<commit_message>
fix fermentation improvements in scenarios C and D
</commit_message>
<xml_diff>
--- a/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_TAL_C.xlsx
+++ b/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_TAL_C.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\Spring 2020\BioSTEAM\Bioindustrial-Park\biorefineries\TAL\analyses\full\parameter_distributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7F0AF1-E486-4A59-9FC4-BAED86AB9374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953E6865-8E5B-4192-82B4-CD1504CD3086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -694,7 +694,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1315,19 +1315,19 @@
         <v>20</v>
       </c>
       <c r="E19" s="6">
-        <v>0.68</v>
+        <v>0.73</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>22</v>
       </c>
       <c r="G19" s="6">
         <f>0.8*E19</f>
-        <v>0.54400000000000004</v>
+        <v>0.58399999999999996</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="6">
         <f>1.2*E19</f>
-        <v>0.81600000000000006</v>
+        <v>0.876</v>
       </c>
       <c r="J19" s="6"/>
       <c r="K19" s="6" t="s">
@@ -1348,19 +1348,19 @@
         <v>12</v>
       </c>
       <c r="E20" s="6">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>22</v>
       </c>
       <c r="G20" s="6">
         <f>E20*0.8</f>
-        <v>60.800000000000004</v>
+        <v>54.400000000000006</v>
       </c>
       <c r="H20" s="6"/>
       <c r="I20" s="6">
         <f>E20*1.2</f>
-        <v>91.2</v>
+        <v>81.599999999999994</v>
       </c>
       <c r="J20" s="6"/>
       <c r="K20" s="6" t="s">

</xml_diff>